<commit_message>
week-2 burndown mistake rectified
</commit_message>
<xml_diff>
--- a/war/CMPE 202 -  Sprint Task Sheet.xlsx
+++ b/war/CMPE 202 -  Sprint Task Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mapka\git repo\sp19-202-cavka\war\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91401662-36EF-4EF5-8969-3EDF91785A14}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1432F32-A52C-4D68-B8AE-9E5D0532E6B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1498,7 +1498,7 @@
   <dimension ref="A1:AG998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+      <selection activeCell="S5" sqref="S5:X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>